<commit_message>
nouvelle version bee boy avec recherche
</commit_message>
<xml_diff>
--- a/commentaire.xlsx
+++ b/commentaire.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vincienergies-my.sharepoint.com/personal/ismail_kallel_vinci-energies_net/Documents/Bureau/bee_boy_2/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_24718A291E477C0E62355476585DCE3A8747069B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B67E4B5E-B43F-45BF-AE42-0F7DA77B9CD3}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>Question</t>
   </si>
@@ -34,166 +28,40 @@
     <t>Avis</t>
   </si>
   <si>
-    <t>panne avec l'asea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-- Defaut colmatage filtre + temperature huile basse, impossible de demarrer pompe HP1 et HP2 
-- Extinction de la clim, relance NOK toujours le meme defaut. 
-- Laissé la clim eteinte quelques minutes (20 min) 
-- Relance ok , les moteurs se sont mis en marche 
-- Rallumage de la clim prevu dans 1 heures 
-- Recherche aspirateur
-- Essai de l'aspirateur qui est entre les deux armoires électriques des machines à coté de la salle insonorisée et il fonctionne.
-- Forcage de la decompression table sur pupitre ok 
-- Le niveau est passé de 70% à 75% 
-- Remis l'appoint avec SUEZ (78%) 
-- Nettoyage des taches d'huile dans le local 
-- Fait plusieurs cycle en auto ok, le niveau remonte bien à 78% 
-- Rendu en prod</t>
-  </si>
-  <si>
-    <t>merci c'est tres utile</t>
-  </si>
-  <si>
-    <t>j'ai une panne dans la fms42</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 
-- Vu avec ope, bon traité par MI sur aspiration machine
-- Recherche aspirateur et opérateur
-- Changement d'équipe et les autres opérateurs ne le connaissent visiblement pas
-- Essai de l'aspirateur qui est entre les deux armoires électriques des machines à coté de la salle insonorisée et il fonctionne
-- Remis en configuration Ok
-- Essaie avec opérateur OK
-- Rendu en prod
-- Control dans l'armoir élèc
-- Le thermique des rideaux a déclenché
-- Rearmement OK
-- Essaie avec op OK
-- Rendu en prod
-- Relance du cycle Ok
-- Essaie Ok
-- Rendu en prod
-- à notre arrivée, aucun défaut sur la machine
-- essais mouvements en Z ras
-- vu avec op, il a eu les défauts de graissage en Z1 et Z2
-- nous ras
-- relance prog avec op ok 
-- rendue
-- remis en condition
-- relance &gt;&gt; ok
-- essai entree sortir palette &gt;&gt;ok  
-- surveillance 1h sans defaut ( 6 ordres sortir retour palette) &gt;&gt;ok.
-- rendu en prod
-- Remis en configuration Ok
-- Relance du cycle Ok
-- Essaie Ok
-- Rendu en prod
-- Controle du codeur 
-- Controle du capteur de POM 
-- Par contre il ne compte que deux plateaux et si on essai d\'en appeler un autre il dit " plateau inconnu "
-- faire intervenir KARDEX
-- envoyé un mail a kardex pour une demande d\'intervention
-- Intervention de kardex le kardex est rendu au nominal l\'apprentissage des tiroirs est OK
-- cloture du bon
-- Pression controlé à 65 bars ok
-- cloture du bon de panne
-- traité sur le bon de panne du 31.07.2022
-- Doublon, bon de panne jumeau cloturé le jour d'après
-- L'opérateur a redémarré l'IHM et il fonctionne. Plus de problème.
-- Panne général. OEE à nouveau focntionnel.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reponse moyennne </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> POUR CHAQUE ELEMENTS
-- Contrôle du niveau d'huile et remise en configuration OK 
-- Recherche de fuite 
-- Beaucoup d'huile présente dans le tunnel entre le magasin et la presse 
-- Présence d'huile sous la table coté A
-- Forcage de la décompression table sur pupitre 
-- Remis l'appoint avec SUEZ 
-- Nettoyage des taches d'huile dans le local 
-- Réalisation sous OT pour tampons 
-- Contrôle dans l'armoire électrique 
-- Réarmement OK 
-- Essai avec opérateur OK 
-- Rendu en production</t>
-  </si>
-  <si>
-    <t>merci pour cette reponse utile</t>
-  </si>
-  <si>
-    <t>j'ai une panne avec l'asea</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 
-- Defaut colmatage filtre + temperature huile basse, impossible de demarrer pompe HP1 et HP2 
-- Extinction de la clim, relance NOK toujours le meme defaut. 
-- Laissé la clim eteinte quelques minutes (20 min) 
-- Relance ok , les moteurs se sont mis en marche 
-- Rallumage de la clim prevu dans 1 heures 
-- Remis en configuration Ok  
-- Essaie avec opérateur OK  
-- Rendu en prod 
-- Control dans l'armoir élèc  
-- Le thermique des rideaux a déclenché  
-- Rearmement OK  
-- Essaie avec op OK  
-- Rendu en prod 
-- à notre arrivée, aucun défaut sur la machine 
-- essais mouvements en Z ras 
-- vu avec op, il a eu les défauts de graissage en Z1 et Z2 
-- nous ras 
-- relance prog avec op ok 
-- rendue 
-- Sortie table avec le treuil 
-- les sorties sont bien pilotées sur le bloc foré 
-- la pression varie bien sur l'IHM. 
-- le problème semble venir des electrovannes sur le bloc foré.  
-- Control de toutes les gaches de sécurités Ok   
-- Control du PAD, il est bombé comme si il y avait encore de l'huile 
-- Vidange forcé de l'huile dans le pad 
-- Essaie de rentré / sortie des deux tables OK 
-- Fait 7 cycles de presse avec l'opérateur Ok   
-- Moyen rendu en prod 
-- Pression controlé à 65 bars ok 
-- traité sur le bon de panne du 31.07.2022 
-- resset le défaut ok 
-- rendu 
-- Opérateur pas au courant de la panne... 
-- Moyen rendu 
-- L'opérateur a redémarré l'IHM et il fonctionne. Plus de problème. 
-- OEE à nouveau focntionnel.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">merci pour cette reponse </t>
-  </si>
-  <si>
-    <t xml:space="preserve">j'ai une panne sur l'asea </t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-- Défaut colmatage filtre + temperature huile basse, impossible de demarrer pompe HP1 et HP2 
-- Extinction de la clim, relance NOK toujours le meme défaut. 
-- Laissé la clim éteinte quelques minutes (20 min) 
-- Relance ok , les moteurs se sont mis en marche 
-- Rallumage de la clim prévu dans 1 heures 
-- Recherche aspirateur 
-- Essai de l'aspirateur qui est entre les deux armoires électriques des machines à coté de la salle insonorisée et il fonctionne 
-- Forçage de la décompression table sur pupitre ok 
-- Remis l'appoint avec SUEZ (78%) 
-- Nettoyage des taches d'huile dans le local 
-- Fait plusieurs cycle en auto ok, le niveau remonte bien à 78% 
-- Rendu en production.</t>
-  </si>
-  <si>
-    <t>oui c'est ca merci</t>
-  </si>
-  <si>
     <t>panne sur la 4ta 4 erreur erreur syncro</t>
+  </si>
+  <si>
+    <t>panne sur la fms41 magasin bloqué</t>
+  </si>
+  <si>
+    <t>panne sur la tandem 2 erreur changement d'outil</t>
+  </si>
+  <si>
+    <t>panne sur la tandem changement d'outil</t>
+  </si>
+  <si>
+    <t>panne avec la tandem</t>
+  </si>
+  <si>
+    <t>panne changement d'outil avec la tandem 2</t>
+  </si>
+  <si>
+    <t>fuite d'air sackee</t>
+  </si>
+  <si>
+    <t>panne de pression d'air sur la saackee 3</t>
+  </si>
+  <si>
+    <t>panne asea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">panne de paletisation fms42 </t>
+  </si>
+  <si>
+    <t>panne sur bord sensible de la machine v4</t>
+  </si>
+  <si>
+    <t>c'est quoi les logins</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -208,12 +76,6 @@
 - Resserage des vis.</t>
   </si>
   <si>
-    <t>oui</t>
-  </si>
-  <si>
-    <t>panne sur la fms41 magasin bloqué</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 - déblocage du magasin et relance cycle ok
 - Remis en configuration Ok, essaie avec opérateur ok et mise en production
@@ -221,12 +83,6 @@
 - Remis en condition du bras chargeur de meule, essais avec opérateur OK et mise en production
 - Shunt des securités et remise en état en mode manu, retour en auto NOK et remise en condition en manu
 - Vérification de la position du chariot dans le magasin ok, cycle terminé, vérification des doigts ok, coupure du magasin puis relance et mise en production</t>
-  </si>
-  <si>
-    <t>c'est bien pour le moment</t>
-  </si>
-  <si>
-    <t>panne sur la tandem 2 erreur changement d'outil</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -247,12 +103,6 @@
 - Moyen rendu en production. 
 - Remis en etat en mode manu Retour en auto NOK On a du rentrer le cube en manu Refais cycle en auto ok. 
 - Rendu en prod.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c'est pas en relation avec la question posée, je crois c'est en relation avec les chiffres dans la question </t>
-  </si>
-  <si>
-    <t>panne sur la tandem changement d'outil</t>
   </si>
   <si>
     <t xml:space="preserve"> ENTRE LES ACTIONS 
@@ -278,12 +128,6 @@
 • Réamorçage pompe lub, essais OK, rendu en prod.</t>
   </si>
   <si>
-    <t>c'est pas bon</t>
-  </si>
-  <si>
-    <t>panne avec la tandem</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 -Vu avec ope, bon traité par MI sur aspiration machine
 -Recherche aspirateur et opérateur 
@@ -304,12 +148,6 @@
 -L'opérateur a redémarré l'IHM et il fonctionne.</t>
   </si>
   <si>
-    <t>c'est pas bon aussi , voir l'exemple de la tandem</t>
-  </si>
-  <si>
-    <t>panne changement d'outil avec la tandem 2</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 - Arrêt d'urgence du variateur de la porte gauche
 - Mise à jour logicielle de la machine en attente
@@ -317,9 +155,6 @@
 - Changer l'outil avec la tândem 2</t>
   </si>
   <si>
-    <t>toujours un probleme avec la tandem</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 - Vérifié le défaut avec un opérateur
 - Arrêter la machine à la fin de poste, avec les tables à l'extérieur de la machine 
@@ -327,14 +162,133 @@
 - Changement d'outil avec la Tandem 2</t>
   </si>
   <si>
+    <t xml:space="preserve"> - Réparation de la fuite d'air 
+- Vérification du réglage du petit distributeur monté sur le vérin 
+- Relance cycle 
+- Démontage et remplacement du joint au silicone 
+- Remplacement de l'enrouleur 
+- Rempacement de l'embout 
+- Remplacement du Staubli et raccord 
+- Test et recontrôle de l'étanchéité 
+- Grattage et nettoyage de la ridelle et de la table, remontage et étanchéité de la ridelle, séchage 
+- Remplacement du corps de pistolet, de la vanne d'alimentation en air et de la brosse 
+- Remplacement du raccord pneumatique 
+- Essai final</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1. Vérifié et ajusté la pression sortant de la saackee 3 si nécessaire.
+2. Examiner la pipeline d'air pour rechercher des fuites et les réparer si nécessaire. 
+3. Régler ou remplacer les pièces défectueuses ou usées si nécessaire.
+4. Vérifier le fonctionnement des vannes et les nettoyer si nécessaire.
+5. Remplacer ou ajuster la soupape de sécurité si nécessaire.
+6. Contrôler le filtre à air pour vérifier qu'il n'est pas obstrué. 
+7. Contrôler les niveaux de lubrification des composants en mouvement et vérifier s'ils sont adéquats.
+8. Régler ou remplacer les roulements, les joints d'étanchéité, les pompes, les connexions et les bouchons des raccords à pression si nécessaire.
+9. Vérifier que les conduits de pression du système sont correctement ancrés.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> HS
+1. Controle des pressostats PS4A, PS4B
+2. Resserage des connectiques
+3. Control du distributeur V10B
+4. Rearmement
+5. Fait 4 cycles avec l'opérateur
+6. Controle de la température du groupe hydraulique 
+7. Controle de la température dans la salle
+8. Tests OK en prod 
+9. Relance de la presse
+10. Réalisation du sous-ot pour le filtre en question
+11. Remplacement du filtre
+12. Laissé le moteur tourner un peu afin de vérifier s'il y a une leakage
+13. Validation et rendu en production
+14. Remise en place de la porte
+15. Contactation CE chef de production pour effectuer MyFM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+• Remise en condition initiale et nettoyage de l'embase 
+• Contrôle des coupleurs et des capteurs des coupleurs 
+• Nettoyage du vérin de verrou palet 
+• Retrait des copeaux pour permettre la détection du capteur 
+• Nettoyage et prise de référence 
+• Relance de plusieurs chargements/déchargements palets 
+• Contrôle de la porte 
+• Shunt sécurité 
+• Remise en configuration initiale 
+• Essai 
+• Contrôle des coupleurs 
+• Remise en configuration de la palettisation 
+• Relance cycle palettisation 
+• Modification de la cote en Z pour le FMS42 
+• Réglage des détecteurs des centreurs bas 
+• Test sortie palet m62 
+• Reset du défaut 
+• Palletisation 
+• Remise en cycle de la palettisation 
+• Remise en place de la prise d'alimentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 
+• Planification d’une vérification complète et approfondie de la machine V4. 
+• Contrôle des disques durs et du système d'exploitation pour rechercher des erreurs ou des anomalies.  
+• Analyse du système pour déterminer l’état des composants.
+• Vérification des branchements et connexions électriques pour s'assurer qu'ils sont corrects.
+• Examen du registre d’événements système pour trouver des informations de diagnostic sur la panne. 
+• Analyse des performances et des informations du processeur pour examiner son état.
+• Analyse logicielle et matérielle pour identifier les composants défectueux.
+• Dépannage des problèmes matériels et recherche de solutions. 
+• Restauration et réinitialisation des paramètres par défaut de la machine V4. 
+• Mise à jour des logiciels et des pilotes appropriés pour améliorer les performances de la machine.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> et passwords ?
+Les logins et passwords sont : Identifiant: 752, Mot de passe: 752</t>
+  </si>
+  <si>
+    <t>oui</t>
+  </si>
+  <si>
+    <t>c'est bien pour le moment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c'est pas en relation avec la question posée, je crois c'est en relation avec les chiffres dans la question </t>
+  </si>
+  <si>
+    <t>c'est pas bon</t>
+  </si>
+  <si>
+    <t>c'est pas bon aussi , voir l'exemple de la tandem</t>
+  </si>
+  <si>
+    <t>toujours un probleme avec la tandem</t>
+  </si>
+  <si>
     <t>probleme avec la tandem car dans la description des autres panne il donne l'exemple de la tandem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c'est pas mal en gros, </t>
+  </si>
+  <si>
+    <t>il manque l'action:
+il faut ouvrir et fermer les portes 
+apres demarrage</t>
+  </si>
+  <si>
+    <t>la premiere partie est bonne la 2eme n'est pas sur la bonne machine</t>
+  </si>
+  <si>
+    <t>il ya seuleme,nt une seule action qui est bonne</t>
+  </si>
+  <si>
+    <t>tres bonne reponse</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -345,7 +299,10 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -394,14 +351,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -689,19 +638,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="49.88671875" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -715,7 +659,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -723,237 +667,217 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="E2">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="E3">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="E4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="E5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="E6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="E7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="E8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="E9">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="E10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
         <v>25</v>
       </c>
-      <c r="D11" t="s">
-        <v>26</v>
-      </c>
       <c r="E11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="E12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="E13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update commentaire et requirements
</commit_message>
<xml_diff>
--- a/commentaire.xlsx
+++ b/commentaire.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
   <si>
     <t>Question</t>
   </si>
@@ -68,6 +68,15 @@
   </si>
   <si>
     <t>quelle est la procédure pour refaire le zéro du Z</t>
+  </si>
+  <si>
+    <t>les seuils ph?</t>
+  </si>
+  <si>
+    <t>donne moi la procedure complete en details su le reglage du ph</t>
+  </si>
+  <si>
+    <t>donne moi les login et mot de passe pour chaque machiine</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -260,6 +269,27 @@
 La procédure pour refaire le zéro du Z dans le problème 102319462 consiste à vérifier le 0 du W, à régler le 0 du Z, à lancer le datum et à contrôler et régler de nouveau si le datum ne passe pas.</t>
   </si>
   <si>
+    <t xml:space="preserve"> 
+Il n'y a pas de seuils PH spécifiés dans ces données. Les données indiquent que le PH devrait être à 9 et que l'electrode doit être changée pour voir s'il y a du mieux. L'étalonnage doit également être effectué avec SUEZ, et des bidons PH4, PH7 et PH9 doivent être bas pour cela.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> de la cuve
+Procédure pour le réglage du PH de la cuve : 
+1. Préparation pour l'étalonnage - Remplir le bidon avec du PH 4, du PH 7 et du PH 9 et placer les fioles pour l'étalonnage en bas. Disposer la pipette demi-eau en bas également.
+2. Monter la sonde et procéder à l'étalonnage - Monter la sonde et procéder à l'étalonnage selon les instructions de Suez.
+3. Connexion et remise en place du tout - Effectuer la connexion et assurer la remise en place du tout.
+4. Attente de la remise en température des cuves à 52°C - Attendre que la température des cuves atteigne les 52°C pour procéder à l'essai avec l'opérateur.
+5. Essais avec l'opérateur - Procéder aux essais avec l'opérateur selon les instructions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Pour la machine 5295 : Utilisateur: 123  Mot de passe: 321
+Pour la machine 51783 : Utilisateur: 752  Mot de passe: 752
+Pour la machine 5232 : Aucun login et mot de passe spécifiés
+Pour la machine 5252 : Aucun login et mot de passe spécifiés
+Pour la machine 5304 : Utilisateur: 752  Mot de passe: 752</t>
+  </si>
+  <si>
     <t>oui</t>
   </si>
   <si>
@@ -303,6 +333,12 @@
   <si>
     <t xml:space="preserve">réponse precise
 </t>
+  </si>
+  <si>
+    <t>yess</t>
+  </si>
+  <si>
+    <t>tres bonne reponse merci</t>
   </si>
 </sst>
 </file>
@@ -660,7 +696,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -688,10 +724,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E2">
         <v>4</v>
@@ -705,10 +741,10 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="E3">
         <v>4</v>
@@ -722,10 +758,10 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -739,10 +775,10 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -756,10 +792,10 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -773,10 +809,10 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -790,10 +826,10 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -807,10 +843,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="E9">
         <v>4</v>
@@ -824,10 +860,10 @@
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -841,7 +877,7 @@
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E11">
         <v>4</v>
@@ -855,10 +891,10 @@
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E12">
         <v>3</v>
@@ -872,10 +908,10 @@
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E13">
         <v>2</v>
@@ -889,10 +925,10 @@
         <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D14" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E14">
         <v>5</v>
@@ -906,10 +942,10 @@
         <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="E15">
         <v>5</v>
@@ -923,12 +959,63 @@
         <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D16" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="E16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19">
         <v>5</v>
       </c>
     </row>

</xml_diff>